<commit_message>
Testing BIG and testing name work
</commit_message>
<xml_diff>
--- a/Testbig.xlsx
+++ b/Testbig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ffd71fb06e3113a/Documenten/Python sandbox/Webscraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_E385FE82066CF47EE110B0775C33BEFAADA6968A" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C9F7D4F7-CA32-4ED1-9C8C-1B105A793E02}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_E3850EFA074028AE692920B7575986BEB474EAD1" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A2988145-0204-407E-AD69-05A65B485E8C}"/>
   <bookViews>
     <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +73,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -94,14 +100,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -419,15 +426,15 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C2" sqref="C2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -445,13 +452,14 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>99924036101</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
@@ -460,7 +468,8 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
@@ -469,7 +478,8 @@
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tkinter testing in progress
</commit_message>
<xml_diff>
--- a/Testbig.xlsx
+++ b/Testbig.xlsx
@@ -1,91 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ffd71fb06e3113a/Documenten/Python sandbox/Webscraper/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_E3850EFA074028AE692920B7575986BEB474EAD1" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A2988145-0204-407E-AD69-05A65B485E8C}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blad1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>BIG</t>
-  </si>
-  <si>
-    <t>Achternaam</t>
-  </si>
-  <si>
-    <t>Uitkomst BIG</t>
-  </si>
-  <si>
-    <t>Uitkomst Achternaam</t>
-  </si>
-  <si>
-    <t>Franken</t>
-  </si>
-  <si>
-    <t>Jansen</t>
-  </si>
-  <si>
-    <t>Nepnaam</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <color rgb="FF808080"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0099CC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,29 +84,91 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -422,67 +468,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="4" customWidth="1"/>
+    <col width="13.33203125" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="27.44140625" customWidth="1" style="4" min="2" max="2"/>
+    <col width="27.109375" customWidth="1" style="4" min="3" max="3"/>
+    <col width="19.33203125" customWidth="1" style="4" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>BIG</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Achternaam</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Uitkomst BIG</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Uitkomst Achternaam</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3">
+    <row r="2">
+      <c r="A2" s="3" t="n">
         <v>99924036101</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Franken</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>BIG is geldig, maar geen huisarts</t>
+        </is>
+      </c>
+      <c r="D2" s="7" t="inlineStr">
+        <is>
+          <t>Naam komt overeen</t>
+        </is>
+      </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>19059287401</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Jansen</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>BIG is gekoppeld aan huisarts</t>
+        </is>
+      </c>
+      <c r="D3" s="7" t="inlineStr">
+        <is>
+          <t>Naam komt overeen</t>
+        </is>
+      </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>59919419602</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Nepnaam</t>
+        </is>
+      </c>
+      <c r="C4" s="8" t="inlineStr">
+        <is>
+          <t>BIG levert geen resultaat op</t>
+        </is>
+      </c>
+      <c r="D4" s="8" t="inlineStr">
+        <is>
+          <t>Naam komt niet overeen</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>